<commit_message>
egy két cucc cuccmóklása
</commit_message>
<xml_diff>
--- a/BeadandóKövetelményStatikusWeboldal.xlsx
+++ b/BeadandóKövetelményStatikusWeboldal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2024-2025\webprog\projektmunka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2024-2025\webprog\projektmunka\vxxcbffdg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0EC0BC-E2CE-4793-9081-A98BD65EBE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73ABFB-A15E-400A-819D-EA82CD3D2487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,14 +880,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -981,7 +981,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -993,7 +993,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1069,11 +1069,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,7 +1097,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1105,11 +1105,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D41" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D41" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="D42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="D42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8801,7 +8801,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8820,15 +8820,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
     </row>
@@ -8929,10 +8929,10 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="51">
         <f>COUNTA(Irányelvek!C:C)-1</f>
         <v>41</v>
@@ -8948,10 +8948,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="51">
         <f>SUM(Irányelvek!G:G)</f>
         <v>70</v>
@@ -8965,10 +8965,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="60"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="51">
         <v>30</v>
       </c>
@@ -8981,10 +8981,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="60"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="51">
         <v>10</v>
       </c>
@@ -8997,10 +8997,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="60"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="51">
         <v>30</v>
       </c>
@@ -9027,10 +9027,10 @@
     </row>
     <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="60"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="51" t="b">
         <f t="array" ref="D15">IF(COUNTIFS(Irányelvek!D2:D42,"=hamis",Irányelvek!F2:F42,"=Igaz")=0,TRUE,FALSE)</f>
         <v>0</v>
@@ -9044,13 +9044,13 @@
     </row>
     <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="54">
         <f>SUM(Irányelvek!H2:H42)</f>
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E16" s="52"/>
       <c r="F16" s="70" t="str">
@@ -9081,10 +9081,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="57"/>
       <c r="E18" s="52"/>
       <c r="F18" s="70"/>
@@ -9095,13 +9095,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="54">
         <f>SUM(D16:D18)</f>
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E19" s="52"/>
       <c r="F19" s="61" t="str">
@@ -9128,6 +9128,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GY0qzS23AjeU4FiVxM6V6yTeqAyuwIwkf0prt1k9kjvXMb2kI4aIbHicosNGGfE24sgSmE5PyGQO+AcVTCjtsg==" saltValue="Ta2LPohq4QT75tLdf5jIUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="F16:H18"/>
+    <mergeCell ref="F9:H13"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B1:H1"/>
@@ -9144,8 +9146,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F16:H18"/>
-    <mergeCell ref="F9:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:D19">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -9167,8 +9167,8 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9611,7 +9611,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="22" t="b">
         <v>0</v>
@@ -9620,9 +9620,9 @@
       <c r="G13" s="2">
         <v>1</v>
       </c>
-      <c r="H13" s="15" t="str">
+      <c r="H13" s="15">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I13" s="16" t="str">
         <f t="shared" si="1"/>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="J13" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -9710,7 +9710,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="22" t="b">
         <v>0</v>
@@ -9719,9 +9719,9 @@
       <c r="G16" s="2">
         <v>1</v>
       </c>
-      <c r="H16" s="15" t="str">
+      <c r="H16" s="15">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I16" s="16" t="str">
         <f t="shared" si="1"/>
@@ -9729,7 +9729,7 @@
       </c>
       <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9875,7 +9875,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="22" t="b">
         <v>0</v>
@@ -9884,9 +9884,9 @@
       <c r="G21" s="2">
         <v>1</v>
       </c>
-      <c r="H21" s="15" t="str">
+      <c r="H21" s="15">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I21" s="16" t="str">
         <f t="shared" si="1"/>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="J21" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -10273,7 +10273,7 @@
         <v>7</v>
       </c>
       <c r="D33" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="25" t="b">
         <v>0</v>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="H33" s="15">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="16">
         <f t="shared" si="1"/>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="J33" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -10308,7 +10308,7 @@
         <v>53</v>
       </c>
       <c r="D34" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="27" t="b">
         <v>0</v>
@@ -10321,7 +10321,7 @@
       </c>
       <c r="H34" s="15">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="16">
         <f t="shared" si="1"/>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="J34" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10514,7 +10514,7 @@
         <v>57</v>
       </c>
       <c r="D40" s="28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="22" t="b">
         <v>0</v>
@@ -10527,7 +10527,7 @@
       </c>
       <c r="H40" s="15">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I40" s="16">
         <f t="shared" si="1"/>
@@ -10535,7 +10535,7 @@
       </c>
       <c r="J40" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10549,7 +10549,7 @@
         <v>56</v>
       </c>
       <c r="D41" s="23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="22" t="b">
         <v>0</v>
@@ -10562,7 +10562,7 @@
       </c>
       <c r="H41" s="15">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I41" s="16">
         <f t="shared" si="1"/>
@@ -10570,7 +10570,7 @@
       </c>
       <c r="J41" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10584,7 +10584,7 @@
         <v>22</v>
       </c>
       <c r="D42" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="22" t="b">
         <v>0</v>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="H42" s="15">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I42" s="16">
         <f t="shared" si="1"/>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="J42" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
na már 100% tanárúr nagyon jó
</commit_message>
<xml_diff>
--- a/BeadandóKövetelményStatikusWeboldal.xlsx
+++ b/BeadandóKövetelményStatikusWeboldal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2024-2025\webprog\projektmunka\vxxcbffdg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkkmi\Documents\Suli\projektmunka yefrgthtzjukfjdhrg\vxxcbffdg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D9736A-4BCB-461C-96F7-5E4CFADCE968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98EDB7-39B3-4348-8A67-CB8FFB53A049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>Neved:</t>
   </si>
@@ -322,6 +322,12 @@
       <t>felhasználóval!</t>
     </r>
   </si>
+  <si>
+    <t>Tóth Kata Krisztina, Tóth Zsolt Zétény</t>
+  </si>
+  <si>
+    <t>toth.kata@ckik.hu, toth.zsolt@ckik.hu</t>
+  </si>
 </sst>
 </file>
 
@@ -501,13 +507,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -515,6 +514,12 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -880,22 +885,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -907,6 +896,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -920,6 +912,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1384,9 +1389,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1435,14 +1440,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1471,9 +1476,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1522,14 +1527,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1558,7 +1563,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -1609,14 +1614,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1641,13 +1646,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:rowOff>289560</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>142875</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>247650</xdr:rowOff>
+          <xdr:rowOff>251460</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1696,14 +1701,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1728,13 +1733,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>219075</xdr:rowOff>
+          <xdr:rowOff>220980</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>142875</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>600075</xdr:rowOff>
+          <xdr:rowOff>601980</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1783,14 +1788,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1813,15 +1818,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>137160</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>487680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1870,14 +1875,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1906,7 +1911,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1957,14 +1962,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1993,9 +1998,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2044,14 +2049,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2080,9 +2085,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2131,14 +2136,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2167,9 +2172,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>361950</xdr:rowOff>
+          <xdr:rowOff>365760</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2218,14 +2223,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2254,7 +2259,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2305,14 +2310,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2341,9 +2346,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2392,14 +2397,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2428,7 +2433,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>571500</xdr:rowOff>
         </xdr:to>
@@ -2479,14 +2484,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2515,7 +2520,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -2566,14 +2571,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2602,9 +2607,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2653,14 +2658,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2689,9 +2694,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2740,14 +2745,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2776,7 +2781,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2827,14 +2832,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2863,9 +2868,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>523875</xdr:rowOff>
+          <xdr:rowOff>525780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2914,14 +2919,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2950,9 +2955,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3001,14 +3006,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3037,7 +3042,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3088,14 +3093,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3124,9 +3129,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3175,14 +3180,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3211,7 +3216,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3262,14 +3267,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3298,9 +3303,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3349,14 +3354,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3385,7 +3390,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3436,14 +3441,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3472,9 +3477,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3523,14 +3528,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3559,9 +3564,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3610,14 +3615,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3646,9 +3651,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3697,14 +3702,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3733,7 +3738,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
@@ -3784,14 +3789,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3820,7 +3825,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3871,14 +3876,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3907,9 +3912,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3958,14 +3963,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3994,9 +3999,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>352425</xdr:rowOff>
+          <xdr:rowOff>350520</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4045,14 +4050,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4081,9 +4086,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>390525</xdr:rowOff>
+          <xdr:rowOff>388620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4132,14 +4137,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4168,9 +4173,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4219,14 +4224,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4255,7 +4260,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4306,14 +4311,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4342,9 +4347,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4393,14 +4398,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4429,9 +4434,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4480,14 +4485,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4516,7 +4521,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4567,14 +4572,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4603,9 +4608,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>38</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4654,14 +4659,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4690,7 +4695,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4741,14 +4746,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4773,13 +4778,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>323850</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4828,14 +4833,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4864,7 +4869,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>42</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4915,14 +4920,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4953,7 +4958,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5002,14 +5007,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5040,7 +5045,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5089,14 +5094,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5176,14 +5181,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5206,15 +5211,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>7620</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>314325</xdr:rowOff>
+          <xdr:rowOff>312420</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>276225</xdr:rowOff>
+          <xdr:rowOff>274320</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5263,14 +5268,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5293,15 +5298,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>714375</xdr:colOff>
+          <xdr:colOff>716280</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>219075</xdr:rowOff>
+          <xdr:rowOff>220980</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>142875</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>600075</xdr:rowOff>
+          <xdr:rowOff>601980</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5350,14 +5355,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5382,7 +5387,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -5437,14 +5442,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5524,14 +5529,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5562,7 +5567,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5611,14 +5616,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5649,7 +5654,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5698,14 +5703,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5736,7 +5741,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>361950</xdr:rowOff>
+          <xdr:rowOff>365760</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5785,14 +5790,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5872,14 +5877,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5910,7 +5915,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5959,14 +5964,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6046,14 +6051,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6133,14 +6138,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6171,7 +6176,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6220,14 +6225,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6258,7 +6263,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6307,14 +6312,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6394,14 +6399,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6432,7 +6437,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>523875</xdr:rowOff>
+          <xdr:rowOff>525780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6481,14 +6486,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6519,7 +6524,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6568,14 +6573,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6655,14 +6660,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6693,7 +6698,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6742,14 +6747,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6829,14 +6834,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -6867,7 +6872,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6916,14 +6921,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7003,14 +7008,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7041,7 +7046,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7090,14 +7095,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7128,7 +7133,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7177,14 +7182,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7215,7 +7220,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7264,14 +7269,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7351,14 +7356,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7438,14 +7443,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7476,7 +7481,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7525,14 +7530,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7612,14 +7617,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7650,7 +7655,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>390525</xdr:rowOff>
+          <xdr:rowOff>388620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7699,14 +7704,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7737,7 +7742,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7786,14 +7791,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7873,14 +7878,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7911,7 +7916,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7960,14 +7965,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -7998,7 +8003,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8047,14 +8052,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8134,14 +8139,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8172,7 +8177,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>38</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8221,14 +8226,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8253,7 +8258,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
@@ -8308,14 +8313,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8338,15 +8343,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:colOff>175260</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:rowOff>297180</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8395,14 +8400,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8482,14 +8487,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="hu-HU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="pl-PL" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -8801,66 +8806,70 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C3" sqref="C3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="9" max="9" width="2.44140625" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52"/>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="52"/>
       <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="C2" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
     </row>
-    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="52"/>
       <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="C3" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
@@ -8872,36 +8881,36 @@
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
     </row>
-    <row r="5" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
     </row>
-    <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="52"/>
-      <c r="B6" s="70" t="str">
+      <c r="B6" s="65" t="str">
         <f>CONCATENATE("Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább ",D11," pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.")</f>
         <v>Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább 30 pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="52"/>
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
@@ -8913,7 +8922,7 @@
       <c r="I7" s="52"/>
       <c r="J7" s="52"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="52"/>
       <c r="B8" s="53" t="s">
         <v>38</v>
@@ -8927,91 +8936,91 @@
       <c r="I8" s="52"/>
       <c r="J8" s="52"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="52"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="61"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="51">
         <f>COUNTA(Irányelvek!C:C)-1</f>
         <v>41</v>
       </c>
       <c r="E9" s="52"/>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
       <c r="I9" s="52"/>
       <c r="J9" s="52"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="52"/>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="51">
         <f>SUM(Irányelvek!G:G)</f>
         <v>70</v>
       </c>
       <c r="E10" s="52"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="52"/>
       <c r="J10" s="52"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="52"/>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="51">
         <v>30</v>
       </c>
       <c r="E11" s="52"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="52"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="61"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="51">
         <v>10</v>
       </c>
       <c r="E12" s="52"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
       <c r="I12" s="52"/>
       <c r="J12" s="52"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="52"/>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="61"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="51">
         <v>30</v>
       </c>
       <c r="E13" s="52"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="52"/>
       <c r="B14" s="53" t="s">
         <v>66</v>
@@ -9025,12 +9034,12 @@
       <c r="I14" s="52"/>
       <c r="J14" s="52"/>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="52"/>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="51" t="b">
         <f t="array" ref="D15">IF(COUNTIFS(Irányelvek!D2:D42,"=hamis",Irányelvek!F2:F42,"=Igaz")=0,TRUE,FALSE)</f>
         <v>0</v>
@@ -9042,78 +9051,78 @@
       <c r="I15" s="52"/>
       <c r="J15" s="52"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="52"/>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="54">
         <f>SUM(Irányelvek!H2:H42)</f>
         <v>63</v>
       </c>
       <c r="E16" s="52"/>
-      <c r="F16" s="58" t="str">
+      <c r="F16" s="68" t="str">
         <f>VLOOKUP(D19,Ponthatárok!$C$3:$D$7,2,TRUE)</f>
         <v>Közepes (3)</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
       <c r="I16" s="52"/>
       <c r="J16" s="52"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="52"/>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="72"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="57">
         <f>IF(D16&gt;D11,VLOOKUP(SUM(Irányelvek!J2:J42),Ponthatárok!G2:H12,2,TRUE),0)</f>
         <v>0</v>
       </c>
       <c r="E17" s="52"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="52"/>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="62"/>
       <c r="D18" s="57"/>
       <c r="E18" s="52"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
       <c r="I18" s="52"/>
       <c r="J18" s="52"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="52"/>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="62"/>
       <c r="D19" s="54">
         <f>SUM(D16:D18)</f>
         <v>63</v>
       </c>
       <c r="E19" s="52"/>
-      <c r="F19" s="64" t="str">
+      <c r="F19" s="58" t="str">
         <f>CONCATENATE("Az önértékelés alapján ",VLOOKUP(D19,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
         <v>Az önértékelés alapján Közepes (3)  érdemjegyet kapnál rá.</v>
       </c>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
       <c r="I19" s="52"/>
       <c r="J19" s="52"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="52"/>
       <c r="B20" s="56"/>
       <c r="C20" s="56"/>
@@ -9128,6 +9137,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GY0qzS23AjeU4FiVxM6V6yTeqAyuwIwkf0prt1k9kjvXMb2kI4aIbHicosNGGfE24sgSmE5PyGQO+AcVTCjtsg==" saltValue="Ta2LPohq4QT75tLdf5jIUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>
@@ -9144,8 +9155,6 @@
     <mergeCell ref="F9:H13"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:D19">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -9167,26 +9176,26 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="54.109375" style="50" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="32" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
       <c r="B1" s="35" t="s">
         <v>4</v>
@@ -9217,7 +9226,7 @@
       </c>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -9252,7 +9261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -9287,7 +9296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="36">
         <v>3</v>
       </c>
@@ -9323,7 +9332,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -9359,7 +9368,7 @@
       </c>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="36">
         <v>5</v>
       </c>
@@ -9394,7 +9403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="39">
         <v>6</v>
       </c>
@@ -9429,7 +9438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36">
         <v>7</v>
       </c>
@@ -9464,7 +9473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39">
         <v>8</v>
       </c>
@@ -9497,7 +9506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>9</v>
       </c>
@@ -9530,7 +9539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="39">
         <v>10</v>
       </c>
@@ -9565,7 +9574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>11</v>
       </c>
@@ -9600,7 +9609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
         <v>12</v>
       </c>
@@ -9633,7 +9642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="36">
         <v>13</v>
       </c>
@@ -9666,7 +9675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="39">
         <v>14</v>
       </c>
@@ -9699,7 +9708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="36">
         <v>15</v>
       </c>
@@ -9732,7 +9741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39">
         <v>16</v>
       </c>
@@ -9765,7 +9774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>17</v>
       </c>
@@ -9798,7 +9807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="39">
         <v>18</v>
       </c>
@@ -9831,7 +9840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36">
         <v>19</v>
       </c>
@@ -9864,7 +9873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="39">
         <v>20</v>
       </c>
@@ -9897,7 +9906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>21</v>
       </c>
@@ -9930,7 +9939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="39">
         <v>22</v>
       </c>
@@ -9963,7 +9972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
         <v>23</v>
       </c>
@@ -9996,7 +10005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="39">
         <v>24</v>
       </c>
@@ -10029,7 +10038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="36">
         <v>25</v>
       </c>
@@ -10062,7 +10071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>26</v>
       </c>
@@ -10095,7 +10104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>27</v>
       </c>
@@ -10128,7 +10137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="39">
         <v>28</v>
       </c>
@@ -10163,7 +10172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>29</v>
       </c>
@@ -10196,7 +10205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>30</v>
       </c>
@@ -10229,7 +10238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>31</v>
       </c>
@@ -10262,7 +10271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="39">
         <v>32</v>
       </c>
@@ -10297,7 +10306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>33</v>
       </c>
@@ -10332,7 +10341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="39">
         <v>34</v>
       </c>
@@ -10365,7 +10374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="36">
         <v>35</v>
       </c>
@@ -10400,7 +10409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="39">
         <v>36</v>
       </c>
@@ -10433,7 +10442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A38" s="36">
         <v>37</v>
       </c>
@@ -10468,7 +10477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="39">
         <v>38</v>
       </c>
@@ -10503,7 +10512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="36">
         <v>39</v>
       </c>
@@ -10538,7 +10547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="39">
         <v>40</v>
       </c>
@@ -10573,7 +10582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="36">
         <v>41</v>
       </c>
@@ -10640,9 +10649,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10662,9 +10671,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10684,7 +10693,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -10702,13 +10711,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:rowOff>289560</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:colOff>144780</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>247650</xdr:rowOff>
+                    <xdr:rowOff>251460</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10724,13 +10733,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
+                    <xdr:rowOff>220980</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:colOff>144780</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>600075</xdr:rowOff>
+                    <xdr:rowOff>601980</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10744,15 +10753,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>30480</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:colOff>137160</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>487680</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10772,7 +10781,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10794,9 +10803,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10816,9 +10825,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10838,9 +10847,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>361950</xdr:rowOff>
+                    <xdr:rowOff>365760</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10860,7 +10869,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -10882,9 +10891,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10904,7 +10913,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>571500</xdr:rowOff>
                   </to>
@@ -10926,7 +10935,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -10948,9 +10957,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10970,9 +10979,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10992,7 +11001,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11014,9 +11023,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>523875</xdr:rowOff>
+                    <xdr:rowOff>525780</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11036,9 +11045,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11058,7 +11067,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11080,9 +11089,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11102,7 +11111,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11124,9 +11133,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11146,7 +11155,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>25</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11168,9 +11177,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11190,9 +11199,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11212,9 +11221,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11234,7 +11243,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </to>
@@ -11256,7 +11265,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11278,9 +11287,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11300,9 +11309,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>352425</xdr:rowOff>
+                    <xdr:rowOff>350520</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11322,9 +11331,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>390525</xdr:rowOff>
+                    <xdr:rowOff>388620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11344,9 +11353,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11366,7 +11375,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11388,9 +11397,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11410,9 +11419,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11432,7 +11441,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11454,9 +11463,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>38</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11476,7 +11485,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>40</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11494,13 +11503,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>323850</xdr:rowOff>
+                    <xdr:rowOff>327660</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11520,7 +11529,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>42</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11544,7 +11553,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11566,7 +11575,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11602,15 +11611,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>7620</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>314325</xdr:rowOff>
+                    <xdr:rowOff>312420</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
+                    <xdr:colOff>160020</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>276225</xdr:rowOff>
+                    <xdr:rowOff>274320</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11624,15 +11633,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>714375</xdr:colOff>
+                    <xdr:colOff>716280</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
+                    <xdr:rowOff>220980</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:colOff>144780</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>600075</xdr:rowOff>
+                    <xdr:rowOff>601980</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11648,7 +11657,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -11698,7 +11707,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11720,7 +11729,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11742,7 +11751,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>361950</xdr:rowOff>
+                    <xdr:rowOff>365760</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11786,7 +11795,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11852,7 +11861,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11874,7 +11883,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11918,7 +11927,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>523875</xdr:rowOff>
+                    <xdr:rowOff>525780</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11940,7 +11949,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11984,7 +11993,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12028,7 +12037,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12072,7 +12081,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12094,7 +12103,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12116,7 +12125,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12182,7 +12191,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12226,7 +12235,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>390525</xdr:rowOff>
+                    <xdr:rowOff>388620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12248,7 +12257,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12292,7 +12301,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12314,7 +12323,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12358,7 +12367,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>38</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12374,7 +12383,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>39</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
@@ -12394,15 +12403,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:rowOff>83820</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:colOff>175260</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:rowOff>297180</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12446,17 +12455,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="10"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
         <v>35</v>
       </c>
@@ -12469,7 +12478,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>100</v>
@@ -12482,7 +12491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="8">
         <v>0.4</v>
       </c>
@@ -12499,7 +12508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <v>0.55000000000000004</v>
       </c>
@@ -12517,7 +12526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>0.7</v>
       </c>
@@ -12535,7 +12544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>0.85</v>
       </c>
@@ -12553,7 +12562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -12571,7 +12580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D8" s="5"/>
       <c r="G8">
         <v>12</v>
@@ -12580,7 +12589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G9">
         <v>14</v>
       </c>
@@ -12588,7 +12597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G10">
         <v>16</v>
       </c>
@@ -12596,7 +12605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G11">
         <v>18</v>
       </c>
@@ -12604,7 +12613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G12">
         <v>20</v>
       </c>
@@ -12612,7 +12621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
   </sheetData>

</xml_diff>